<commit_message>
changed test cases, test scenario, check list for IR, added test cases, test scenario for Jetson
</commit_message>
<xml_diff>
--- a/Тестовые сценарии (web-камера+jetson).xlsx
+++ b/Тестовые сценарии (web-камера+jetson).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Контраст\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB3D8F8-04E3-4C38-A3F5-6D7A7DD7FD9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E2505C-1785-442C-B65D-F0D727F00EB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9990" xr2:uid="{13E3AFFA-99BC-4A72-A9C1-8EB9A3181F0F}"/>
   </bookViews>
@@ -52,40 +52,7 @@
     <t>Проверить работу «Зритель-Контраст» в АРМ ОПК</t>
   </si>
   <si>
-    <t xml:space="preserve">CIR-W S2.0 </t>
-  </si>
-  <si>
-    <t>CIR-W S2.1</t>
-  </si>
-  <si>
-    <t>1. CIR-W0001
-2. CIR-W0002
-3. CIR-W0003
-4. CIR-W0004
-5. CIR-W0005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.2 </t>
-  </si>
-  <si>
     <t>Проверить форму захвата</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.3 </t>
-  </si>
-  <si>
-    <t>Проверить отсутствие графических элементов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Отсутствие в списке «Настройка» пункта «Зритель-Каскад»
-2. Отсутствие демо панели в главной форме </t>
-  </si>
-  <si>
-    <t>1. CIR-W0019
-2. CIR-W0020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.4 </t>
   </si>
   <si>
     <t>Проверить работу горячих клавиш в АРМ ОПК</t>
@@ -96,35 +63,12 @@
 3. Запуск захвата сочетанием клавиш Ctrl + F9</t>
   </si>
   <si>
-    <t>1. CIR-W0021
-2. CIR-W0022
-3. CIR-W0023</t>
-  </si>
-  <si>
     <t>Отключение видоекамеры</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.5 </t>
-  </si>
-  <si>
-    <t>1. CIR-W0024
-2. CIR-W0025
-3. CIR-W0026</t>
   </si>
   <si>
     <t>1. Отключение видеокамеры во время захвата
 2. Кратковременное отключение видеокамеры во время захвата 
 3. Повторный захват после кратковременного отключения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIR-W S2.6 </t>
-  </si>
-  <si>
-    <t>1. CIR-W0036
-2. CIR-W0037
-3. CIR-W0038
-4. CIR-W0039
-5. CIR-W0040</t>
   </si>
   <si>
     <t xml:space="preserve">1. Создание логов «Контраст» при входе в «Система Каскад»
@@ -132,20 +76,6 @@
 3. Начало работы «Контраст» в логах
 4. Конец работы «Контраст» в логах
 5. Инициализация «Контраст-сервиса» </t>
-  </si>
-  <si>
-    <t>1. CIR-W0006
-2. CIR-W0007
-3. CIR-W0008
-4. CIR-W0009
-5. CIR-W0012
-6. CIR-W0016
-7. CIR-W0017
-8. CIR-W0018
-9. CIR-W0027
-10. CIR-W0028
-11. CIR-W0029
-12. CIR-W0041</t>
   </si>
   <si>
     <t>1. Работа «Зритель-контраст» в «АРМ ОПК» 
@@ -162,9 +92,6 @@
 12. Захват кадра на последних секундах таймаута</t>
   </si>
   <si>
-    <t>CIR-W S2.7</t>
-  </si>
-  <si>
     <t>Проверить логи</t>
   </si>
   <si>
@@ -178,33 +105,7 @@
 5. Верификация после захвата в форме захвата</t>
   </si>
   <si>
-    <t>1. CIR-W0046
-2. CIR-W0047
-3. CIR-W0048
-4. CIR-W0049
-5. CIR-W0050</t>
-  </si>
-  <si>
     <t>№</t>
-  </si>
-  <si>
-    <t>1. CIR-W0010
-2. CIR-W0011
-3. CIR-W0013
-4. CIR-W0014
-5. CIR-W0015
-6. CIR-W0030
-7. CIR-W0031
-8. CIR-W0032
-9. CIR-W0033
-10. CIR-W0034
-11. CIR-W0035
-12. CIR-W0042
-13. CIR-W0043
-14. CIR-W0044
-15. CIR-W0045
-16. CIR-W0051
-17. CIR-W0052</t>
   </si>
   <si>
     <t>1. Вызов формы захвата с наличием захваченного кадра
@@ -226,18 +127,7 @@
 17. Захват кадра на большом расстоянии в форме захвата</t>
   </si>
   <si>
-    <t>CIR-W S2.8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Проверить работу камеры в разных ориентациях </t>
-  </si>
-  <si>
-    <t>1. CIR-W0053
-2. CIR-W0054
-3. CIR-W0055
-4. CIR-W0056
-5. CIR-W0057
-6. CIR-W0058</t>
   </si>
   <si>
     <t>1. Захват  в главной форме АРМ ОПК с повернутой на 90 градусов камерой по часовой стрелке
@@ -246,6 +136,122 @@
 4. Захват в форме захвата с повернутой на 180 градусов камерой по часовой стрелке
 5. Захват в главной форме АРМ ОПК с повернутой на 270 градусов камерой по часовой стрелке
 6. Захват в форме захвата с повернутой на 270 градусов камерой по часовой стрелке</t>
+  </si>
+  <si>
+    <t>Проверить стабильность работы после отключений и перезапуска Jetson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-J S2.0 </t>
+  </si>
+  <si>
+    <t>1. CIR-J0001
+2. CIR-J0002
+3. CIR-J0003
+4. CIR-J0004
+5. CIR-J0005</t>
+  </si>
+  <si>
+    <t>CIR-J S2.1</t>
+  </si>
+  <si>
+    <t>1. CIR-J0006
+2. CIR-J0007
+3. CIR-J0008
+4. CIR-J0009
+5. CIR-J0012
+6. CIR-J0016
+7. CIR-J0017
+8. CIR-J0018
+9. CIR-J0025
+10. CIR-J0026
+11. CIR-J0027
+12. CIR-J0039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-J S2.2 </t>
+  </si>
+  <si>
+    <t>1. CIR-J0010
+2. CIR-J0011
+3. CIR-J0013
+4. CIR-J0014
+5. CIR-J0015
+6. CIR-J0028
+7. CIR-J0029
+8. CIR-J0030
+9. CIR-J0031
+10. CIR-J0032
+11. CIR-J0033
+12. CIR-J0040
+13. CIR-J0041
+14. CIR-J0042
+15. CIR-J0043
+16. CIR-J0049
+17. CIR-J0050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-J S2.3 </t>
+  </si>
+  <si>
+    <t>1. CIR-J0019
+2. CIR-J0020
+3. CIR-J0021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR-J S2.4 </t>
+  </si>
+  <si>
+    <t>1. CIR-J0022
+2. CIR-J0023
+3. CIR-J0024</t>
+  </si>
+  <si>
+    <t>CIR-J S2.5</t>
+  </si>
+  <si>
+    <t>1. CIR-J0034
+2. CIR-J0035
+3. CIR-J0036
+4. CIR-J0037
+5. CIR-J0038</t>
+  </si>
+  <si>
+    <t>CIR-J S2.6</t>
+  </si>
+  <si>
+    <t>1. CIR-J0044
+2. CIR-J0045
+3. CIR-J0046
+4. CIR-J0047
+5. CIR-J0048</t>
+  </si>
+  <si>
+    <t>CIR-J S2.7</t>
+  </si>
+  <si>
+    <t>1. CIR-J0051
+2. CIR-J0052
+3. CIR-J0053
+4. CIR-J0054
+5. CIR-J0055
+6. CIR-J0056</t>
+  </si>
+  <si>
+    <t>CIR-J S2.8</t>
+  </si>
+  <si>
+    <t>1. CIR-J0057
+2. CIR-J0058
+3. CIR-J0059
+4. CIR-J0060
+5. CIR-J0061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Отключение Jetson от компьютера после запуска «Система Каскад»
+2. Отключение Jetson от компьютера во время захвата в главной форме АРМ ОПК
+3. Отключение Jetson от компьютера во время захвата в форме захвата
+4. Повторное подключение Jetson после отключения от компьютера
+5. Перезагрузка Jetson с помощью кнопки «Reset» на корпусе </t>
   </si>
 </sst>
 </file>
@@ -325,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -335,6 +341,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -653,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DDC8C5-BDD2-4180-BFE1-6F2E2D051BB8}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E25" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +677,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -688,13 +697,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -705,16 +714,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="284.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -722,112 +731,112 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>39</v>

</xml_diff>